<commit_message>
Add assets folder with images and data
</commit_message>
<xml_diff>
--- a/skillspread_dataset.xlsx
+++ b/skillspread_dataset.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sql, excel, python, data analysis, pandas, statistics, machine learning</t>
+          <t>sql, excel, python, data analysis, pandas, statistics, power bi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>"{\"sql\": {\"free\": \"[Khan Academy \\u2013 SQL](https://www.khanacademy.org/computing/computer-programming/sql)\", \"paid\": \"[Udemy \\u2013 SQL Bootcamp](https://www.udemy.com/course/the-complete-sql-bootcamp/)\"}, \"excel\": {\"free\": \"[Excel Easy](https://www.excel-easy.com/)\", \"paid\": \"[Coursera \\u2013 Google Data Analytics](https://www.coursera.org/professional-certificates/google-data-analytics)\"}, \"python\": {\"free\": \"[freeCodeCamp \\u2013 Python](https://www.freecodecamp.org/learn/)\", \"paid\": \"[Udemy \\u2013 Python Mega Course](https://www.udemy.com/course/the-python-mega-course/)\"}, \"data analysis\": {\"free\": \"[Kaggle Learn \\u2013 Data Analysis](https://www.kaggle.com/learn/pandas)\", \"paid\": \"[Coursera \\u2013 Data Analysis with Python](https://www.coursera.org/learn/data-analysis-with-python)\"}, \"pandas\": {\"free\": \"[Pandas Docs](https://pandas.pydata.org/docs/)\", \"paid\": \"[Udemy \\u2013 Pandas](https://www.udemy.com/course/data-analysis-with-pandas/)\"}, \"statistics\": {\"free\": \"[Khan Academy \\u2013 Statistics](https://www.khanacademy.org/math/statistics-probability)\", \"paid\": \"[Coursera \\u2013 Stanford Statistics](https://www.coursera.org/learn/stanford-statistics)\"}}"</t>
+          <t>"{\"sql\": {\"free\": \"[Khan Academy \\u2013 SQL](https://www.khanacademy.org/computing/computer-programming/sql)\", \"paid\": \"[Udemy \\u2013 SQL Bootcamp](https://www.udemy.com/course/the-complete-sql-bootcamp/)\"}, \"excel\": {\"free\": \"[Excel Easy](https://www.excel-easy.com/)\", \"paid\": \"[Coursera \\u2013 Google Data Analytics](https://www.coursera.org/professional-certificates/google-data-analytics)\"}, \"python\": {\"free\": \"[freeCodeCamp \\u2013 Python](https://www.freecodecamp.org/learn/)\", \"paid\": \"[Udemy \\u2013 Python Mega Course](https://www.udemy.com/course/the-python-mega-course/)\"}, \"data analysis\": {\"free\": \"[Kaggle Learn \\u2013 Data Analysis](https://www.kaggle.com/learn/pandas)\", \"paid\": \"[Coursera \\u2013 Data Analysis with Python](https://www.coursera.org/learn/data-analysis-with-python)\"}, \"pandas\": {\"free\": \"[Pandas Docs](https://pandas.pydata.org/docs/)\", \"paid\": \"[Udemy \\u2013 Pandas](https://www.udemy.com/course/data-analysis-with-pandas/)\"}, \"statistics\": {\"free\": \"[Khan Academy \\u2013 Statistics](https://www.khanacademy.org/math/statistics-probability)\", \"paid\": \"[Coursera \\u2013 Stanford Statistics](https://www.coursera.org/learn/stanford-statistics)\"}, \"power bi\": {\"free\": \"[Microsoft](https://learn.microsoft.com/en-us/training/powerplatform/power-bi)\", \"paid\": \"[Linkedin Learning](https://www.linkedin.com/learning/power-bi-essential-training)\"}}"</t>
         </is>
       </c>
     </row>

</xml_diff>